<commit_message>
Filtering the CSNAPNI to only consider the Chesapeake Bay Watershed (CBW
</commit_message>
<xml_diff>
--- a/OutputFileKeys/CommonDataLabels.xlsx
+++ b/OutputFileKeys/CommonDataLabels.xlsx
@@ -40734,8 +40734,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010050CB5C7BD841A746A008EF8990FEF8A1" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="af3cd4e38eab4ac2fa97473cd31e4822">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d795cf93-200f-4322-ae4e-3af3c2bc7b07" xmlns:ns3="bec3e06c-9dd4-4aa2-90c9-9a788c41bf59" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fa13b4ea85a0338065f13f7b4bcf2fc3" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010050CB5C7BD841A746A008EF8990FEF8A1" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="04f0adbf5da449b72a87907c36bfe402">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d795cf93-200f-4322-ae4e-3af3c2bc7b07" xmlns:ns3="bec3e06c-9dd4-4aa2-90c9-9a788c41bf59" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f5e4044cd58a51a52832fd40a04c970f" ns2:_="" ns3:_="">
     <xsd:import namespace="d795cf93-200f-4322-ae4e-3af3c2bc7b07"/>
     <xsd:import namespace="bec3e06c-9dd4-4aa2-90c9-9a788c41bf59"/>
     <xsd:element name="properties">
@@ -40756,6 +40756,8 @@
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -40820,6 +40822,13 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="28b28469-8996-4088-bd89-44d87d6385e5" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="bec3e06c-9dd4-4aa2-90c9-9a788c41bf59" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -40849,6 +40858,17 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="22" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{68644ca3-003b-4e0e-bb82-ecd3a2033107}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="bec3e06c-9dd4-4aa2-90c9-9a788c41bf59">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -40961,12 +40981,17 @@
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d795cf93-200f-4322-ae4e-3af3c2bc7b07">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="bec3e06c-9dd4-4aa2-90c9-9a788c41bf59" xsi:nil="true"/>
+  </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BDF4331-4A49-4D8D-809A-C581F4077EA8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F2322E5-3ED3-492C-B816-E6923A13299F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
5th Commit | Important Commit
- Create if parameters on settings for grass scenario (unfertilized and fertilized)
- changed some parameters in the code to better represent the number of crops and it to be more soft coded
- Changed the area variable
- added completely grass as a crop
- plugged temporarily change for population for discharge area (new value correct, but make it better coded)*
- added csv files provided from Zia on InputFiles_CBW. This files represent cropscape information to be included soon in the model*
- Rest is just update on files by running the model
</commit_message>
<xml_diff>
--- a/OutputFileKeys/CommonDataLabels.xlsx
+++ b/OutputFileKeys/CommonDataLabels.xlsx
@@ -40734,8 +40734,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010050CB5C7BD841A746A008EF8990FEF8A1" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="04f0adbf5da449b72a87907c36bfe402">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d795cf93-200f-4322-ae4e-3af3c2bc7b07" xmlns:ns3="bec3e06c-9dd4-4aa2-90c9-9a788c41bf59" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f5e4044cd58a51a52832fd40a04c970f" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010050CB5C7BD841A746A008EF8990FEF8A1" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bcac96711073587df0b68b080c708180">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d795cf93-200f-4322-ae4e-3af3c2bc7b07" xmlns:ns3="bec3e06c-9dd4-4aa2-90c9-9a788c41bf59" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="98209c71c39a5a5ad103d397a60c957b" ns2:_="" ns3:_="">
     <xsd:import namespace="d795cf93-200f-4322-ae4e-3af3c2bc7b07"/>
     <xsd:import namespace="bec3e06c-9dd4-4aa2-90c9-9a788c41bf59"/>
     <xsd:element name="properties">
@@ -40758,6 +40758,7 @@
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -40828,6 +40829,11 @@
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="23" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="bec3e06c-9dd4-4aa2-90c9-9a788c41bf59" elementFormDefault="qualified">
@@ -40991,7 +40997,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F2322E5-3ED3-492C-B816-E6923A13299F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDD7A1A1-1802-49FF-BBF6-CDA6E37B719B}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>